<commit_message>
Delete space in cnv 16p12.2 entry
</commit_message>
<xml_diff>
--- a/data/input/cnv_data.xlsx
+++ b/data/input/cnv_data.xlsx
@@ -92,7 +92,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -831,7 +831,7 @@
     <t>WP5510</t>
   </si>
   <si>
-    <t xml:space="preserve">16p12.2 </t>
+    <t>16p12.2</t>
   </si>
   <si>
     <t>Chr16:21950135-22431889</t>
@@ -1026,7 +1026,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1206,7 +1206,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1222,12 +1222,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1329,6 +1335,9 @@
   <cellXfs count="20">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -1344,6 +1353,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1365,21 +1377,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1693,1005 +1699,1005 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="40.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="41.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="34.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="8.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="40.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="41.14785714285715" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="19" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="40.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="40.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="156.75">
-      <c r="A2" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="171.75">
+      <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="45.75">
-      <c r="A3" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="47.25">
+      <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60.75">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="10" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60.75">
-      <c r="A6" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="75">
+      <c r="A6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="11" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="32.25">
-      <c r="A9" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33.75">
+      <c r="A9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="10" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="12" t="s">
+      <c r="I10" s="16"/>
+      <c r="J10" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="60.75">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="11" t="s">
+      <c r="I11" s="16"/>
+      <c r="J11" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60.75">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="10" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="11" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="45.75">
-      <c r="A13" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="47.25">
+      <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="10" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="11" t="s">
+      <c r="I13" s="16"/>
+      <c r="J13" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="58.5">
-      <c r="A14" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="60.75">
+      <c r="A14" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="10" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="32.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="11" t="s">
+      <c r="I15" s="16"/>
+      <c r="J15" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="47.4">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="13" t="s">
         <v>140</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="160.95">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="10" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="11" t="s">
+      <c r="I17" s="16"/>
+      <c r="J17" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="11" t="s">
+      <c r="I18" s="16"/>
+      <c r="J18" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="53.4">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="10" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="11" t="s">
+      <c r="I19" s="16"/>
+      <c r="J19" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="133.2">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="10" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="11" t="s">
+      <c r="I20" s="16"/>
+      <c r="J20" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="10" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="11" t="s">
+      <c r="I21" s="16"/>
+      <c r="J21" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="10" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="11" t="s">
+      <c r="I22" s="16"/>
+      <c r="J22" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="47.4">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16" t="s">
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17" t="s">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18" t="s">
         <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="10" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="J24" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="92.40000000000002">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="10" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="29.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="10" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="10" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="11" t="s">
+      <c r="I27" s="16"/>
+      <c r="J27" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="10" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="11" t="s">
+      <c r="I28" s="16"/>
+      <c r="J28" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="10" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="16"/>
+      <c r="J29" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="10" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="11" t="s">
+      <c r="I30" s="16"/>
+      <c r="J30" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="69">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="10" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="10" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="11" t="s">
+      <c r="I32" s="16"/>
+      <c r="J32" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="10" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="11" t="s">
+      <c r="I33" s="16"/>
+      <c r="J33" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="10" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="18"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="10" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J35" s="11" t="s">
+      <c r="J35" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="10" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H36" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="11" t="s">
+      <c r="I36" s="16"/>
+      <c r="J36" s="13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2711,271 +2717,271 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="102.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="34.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="102.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="75.75">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="22.95">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="61.95000000000001">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45.6">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="76.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="39.6">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="45">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.4">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="35.4">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="68.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="160.95">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="53.4">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="51.6">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="92.40000000000002">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="29.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="69">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="13" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2995,43 +3001,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="6"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data August 2025
</commit_message>
<xml_diff>
--- a/data/input/cnv_data.xlsx
+++ b/data/input/cnv_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maastrichtuniversity-my.sharepoint.com/personal/alexandra_valeanu_maastrichtuniversity_nl/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandra\cnv-data\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{567C6611-41D1-4180-B970-902BAF2F5732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4591FAB5-4DD6-4032-90B2-32CA85E42DE5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC00C353-2AFC-47DD-9CA7-BBFCEA1102F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20544" yWindow="0" windowWidth="20832" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1585,7 +1585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1632,8 +1632,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1660,7 +1659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1668,6 +1667,10 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1977,7 +1980,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1985,7 +1988,8 @@
     <col min="1" max="1" width="34.88671875" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.88671875" style="12" bestFit="1" customWidth="1"/>
@@ -2039,6 +2043,7 @@
       <c r="C2" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="D2" s="28"/>
       <c r="E2" s="8" t="s">
         <v>74</v>
       </c>
@@ -2083,7 +2088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2093,6 +2098,7 @@
       <c r="C4" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="D4" s="28"/>
       <c r="E4" s="8" t="s">
         <v>84</v>
       </c>
@@ -2106,6 +2112,7 @@
       <c r="I4" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="J4" s="29"/>
       <c r="K4" s="9" t="s">
         <v>10</v>
       </c>
@@ -2120,6 +2127,8 @@
       <c r="C5" s="8" t="s">
         <v>88</v>
       </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>89</v>
       </c>
@@ -2146,6 +2155,8 @@
       <c r="C6" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="8" t="s">
         <v>92</v>
       </c>
@@ -2172,6 +2183,8 @@
       <c r="C7" s="8" t="s">
         <v>95</v>
       </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="8" t="s">
         <v>96</v>
       </c>
@@ -2273,6 +2286,7 @@
       <c r="C11" s="8" t="s">
         <v>109</v>
       </c>
+      <c r="D11" s="28"/>
       <c r="E11" s="8" t="s">
         <v>110</v>
       </c>
@@ -2286,6 +2300,7 @@
       <c r="I11" s="9" t="s">
         <v>112</v>
       </c>
+      <c r="J11" s="29"/>
       <c r="K11" s="9" t="s">
         <v>6</v>
       </c>
@@ -2309,6 +2324,7 @@
       <c r="I12" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="J12" s="29"/>
       <c r="K12" s="9" t="s">
         <v>60</v>
       </c>
@@ -2346,6 +2362,8 @@
       <c r="C14" s="8" t="s">
         <v>122</v>
       </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="8" t="s">
         <v>123</v>
       </c>
@@ -2506,6 +2524,9 @@
       <c r="C20" s="8" t="s">
         <v>148</v>
       </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="8" t="s">
         <v>149</v>
       </c>
@@ -2515,6 +2536,7 @@
       <c r="I20" s="9" t="s">
         <v>150</v>
       </c>
+      <c r="J20" s="29"/>
       <c r="K20" s="9" t="s">
         <v>50</v>
       </c>
@@ -2555,6 +2577,7 @@
       <c r="C22" s="8" t="s">
         <v>155</v>
       </c>
+      <c r="D22" s="28"/>
       <c r="G22" s="8" t="s">
         <v>156</v>
       </c>
@@ -2595,7 +2618,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
@@ -2686,6 +2709,8 @@
       <c r="C27" s="8" t="s">
         <v>173</v>
       </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="8" t="s">
         <v>174</v>
       </c>
@@ -2718,6 +2743,7 @@
       <c r="I28" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="J28" s="29"/>
       <c r="K28" s="9" t="s">
         <v>24</v>
       </c>
@@ -2732,6 +2758,7 @@
       <c r="C29" s="8" t="s">
         <v>180</v>
       </c>
+      <c r="D29" s="28"/>
       <c r="E29" s="8" t="s">
         <v>181</v>
       </c>
@@ -2745,6 +2772,7 @@
       <c r="I29" s="9" t="s">
         <v>183</v>
       </c>
+      <c r="J29" s="29"/>
       <c r="K29" s="9" t="s">
         <v>8</v>
       </c>
@@ -2913,13 +2941,14 @@
       <c r="G36" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H36" s="16" t="s">
         <v>224</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="J36" s="29"/>
+      <c r="K36" s="16" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2950,7 +2979,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2999,538 +3028,538 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="27" customWidth="1"/>
-    <col min="3" max="4" width="40.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="27"/>
+    <col min="1" max="1" width="34.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="26" customWidth="1"/>
+    <col min="3" max="4" width="40.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="20" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="24" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>